<commit_message>
Added third location to dataset and computed the RMSE
</commit_message>
<xml_diff>
--- a/stats-results/gps-accuracy/gps_data.xlsx
+++ b/stats-results/gps-accuracy/gps_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgy\Documents\Visual Studio\Python\STATS_GEO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgy\Documents\shield-0.1.2\stats-results\gps-accuracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155657B7-AF1B-487D-BA76-5F8F326D35EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77666E6-F45D-43EE-8F5E-A9572B6FB78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8364E2D-750D-464D-970C-C0CD19124D14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Latitude</t>
   </si>
@@ -53,10 +53,13 @@
     <t>Location</t>
   </si>
   <si>
-    <t>JP Rizal Street, Brgy, Pililla - Jala-Jala - Pakil Rd, Pililla, 1910 Rizal</t>
+    <t>Pineda, Pasig City</t>
   </si>
   <si>
-    <t>147 C. Tolentino Compound Banaag Street Pineda Pasig City</t>
+    <t>Pililla,  Rizal</t>
+  </si>
+  <si>
+    <t>Greenwoods, Pasig City</t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57358295-8687-47A8-BB6A-67C22EE0599A}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32:E61"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62:E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +482,7 @@
         <v>121.33733890000001</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -931,7 +934,7 @@
         <v>121.05823030000001</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1369,10 +1372,463 @@
       </c>
       <c r="E61" s="2"/>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>14.562879000000001</v>
+      </c>
+      <c r="B62" s="1">
+        <v>121.09813800000001</v>
+      </c>
+      <c r="C62" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D62" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>14.562879000000001</v>
+      </c>
+      <c r="B63" s="1">
+        <v>121.098139</v>
+      </c>
+      <c r="C63" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D63" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>14.56288</v>
+      </c>
+      <c r="B64" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C64" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D64" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>14.56288</v>
+      </c>
+      <c r="B65" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C65" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D65" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>14.562881000000001</v>
+      </c>
+      <c r="B66" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C66" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D66" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>14.562882</v>
+      </c>
+      <c r="B67" s="1">
+        <v>121.098141</v>
+      </c>
+      <c r="C67" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D67" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>14.562882</v>
+      </c>
+      <c r="B68" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C68" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D68" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>14.562882</v>
+      </c>
+      <c r="B69" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C69" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D69" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>14.562882999999999</v>
+      </c>
+      <c r="B70" s="1">
+        <v>121.098139</v>
+      </c>
+      <c r="C70" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>14.562882999999999</v>
+      </c>
+      <c r="B71" s="1">
+        <v>121.098139</v>
+      </c>
+      <c r="C71" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D71" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>14.562885</v>
+      </c>
+      <c r="B72" s="1">
+        <v>121.098139</v>
+      </c>
+      <c r="C72" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D72" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>14.562886000000001</v>
+      </c>
+      <c r="B73" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C73" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D73" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>14.562886000000001</v>
+      </c>
+      <c r="B74" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C74" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D74" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>14.562887</v>
+      </c>
+      <c r="B75" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C75" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D75" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>14.562887999999999</v>
+      </c>
+      <c r="B76" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C76" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D76" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>14.562889</v>
+      </c>
+      <c r="B77" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C77" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D77" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>14.562889999999999</v>
+      </c>
+      <c r="B78" s="1">
+        <v>121.09814</v>
+      </c>
+      <c r="C78" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D78" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>14.562891</v>
+      </c>
+      <c r="B79" s="1">
+        <v>121.098141</v>
+      </c>
+      <c r="C79" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D79" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>14.562893000000001</v>
+      </c>
+      <c r="B80" s="1">
+        <v>121.09814299999999</v>
+      </c>
+      <c r="C80" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D80" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>14.562893000000001</v>
+      </c>
+      <c r="B81" s="1">
+        <v>121.098144</v>
+      </c>
+      <c r="C81" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D81" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>14.562894</v>
+      </c>
+      <c r="B82" s="1">
+        <v>121.098144</v>
+      </c>
+      <c r="C82" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D82" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>14.562894</v>
+      </c>
+      <c r="B83" s="1">
+        <v>121.098145</v>
+      </c>
+      <c r="C83" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D83" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B84" s="1">
+        <v>121.098146</v>
+      </c>
+      <c r="C84" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D84" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B85" s="1">
+        <v>121.09814799999999</v>
+      </c>
+      <c r="C85" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D85" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B86" s="1">
+        <v>121.09815</v>
+      </c>
+      <c r="C86" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D86" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B87" s="1">
+        <v>121.098151</v>
+      </c>
+      <c r="C87" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D87" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B88" s="1">
+        <v>121.098151</v>
+      </c>
+      <c r="C88" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D88" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B89" s="1">
+        <v>121.098151</v>
+      </c>
+      <c r="C89" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D89" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>14.562894999999999</v>
+      </c>
+      <c r="B90" s="1">
+        <v>121.098151</v>
+      </c>
+      <c r="C90" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D90" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>14.562894</v>
+      </c>
+      <c r="B91" s="1">
+        <v>121.098151</v>
+      </c>
+      <c r="C91" s="1">
+        <v>14.562817000000001</v>
+      </c>
+      <c r="D91" s="1">
+        <v>121.09808700000001</v>
+      </c>
+      <c r="E91" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:E31"/>
     <mergeCell ref="E32:E61"/>
+    <mergeCell ref="E62:E91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>